<commit_message>
Add the ability to import auto pay days and bill mode
</commit_message>
<xml_diff>
--- a/templates/Account Billing Parameters.xlsx
+++ b/templates/Account Billing Parameters.xlsx
@@ -33,6 +33,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>The day that billing is run for this account. Can only be from 1 – 28.</t>
         </r>
@@ -45,6 +46,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>The number of days after the invoice date that the invoice becomes due. Minimum is 0.
 </t>
@@ -58,6 +60,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>The number of days after due days before the account becomes delinquent. Minimum is 0.</t>
         </r>
@@ -70,6 +73,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>If you want to impose a temporary grace period for a specific user (e.g. you want to push out their delinquency calculation to a future date) enter it here in Y-M-D format (e.g. 2016-06-01)</t>
         </r>
@@ -82,6 +86,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>The number of months this user is billed for at a time. Minimum is 1.</t>
         </r>
@@ -94,6 +99,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Enter 1 if the user is tax exempt, 0 if not.</t>
         </r>
@@ -106,6 +112,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Enter 1 to generate printed invoices for this account, 0 if you don't want to.</t>
         </r>
@@ -115,27 +122,29 @@
       <text>
         <r>
           <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>If the invoice is generated for a day other than the billing day, enter it here. E.g. if you want to bill on the 15</t>
+        </r>
+        <r>
+          <rPr>
             <vertAlign val="superscript"/>
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-          </rPr>
-          <t>If the invoice is generated for a day other than the billing day, enter it here. E.g. if you want to bill on the 15</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>th</t>
         </r>
         <r>
           <rPr>
-            <vertAlign val="superscript"/>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t> and generate an invoice for the 1</t>
         </r>
@@ -144,16 +153,35 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-          </rPr>
-          <t>st</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t> of the billing month, enter '15' in Bill Day and '1' in Separate Invoice Day. Leave this blank if invoices are for the same day as they are generated.</t>
+            <charset val="1"/>
+          </rPr>
+          <t>st of the billing month, enter '15' in Bill Day and '1' in Separate Invoice Day. Leave this blank if invoices are for the same day as they are generated.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>The number of days after invoice generation to run auto pay methods</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Invoice or statement, leave blank to use system default</t>
         </r>
       </text>
     </comment>
@@ -162,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Account ID</t>
   </si>
@@ -189,6 +217,12 @@
   </si>
   <si>
     <t>Separate Invoice Day </t>
+  </si>
+  <si>
+    <t>Auto Pay Days</t>
+  </si>
+  <si>
+    <t>Bill Mode</t>
   </si>
 </sst>
 </file>
@@ -203,6 +237,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -235,12 +270,14 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -387,25 +424,25 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>50040</xdr:colOff>
+      <xdr:colOff>77040</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>9720</xdr:rowOff>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>792720</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19440</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:rowOff>105120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvPr id="0" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="50040" y="9720"/>
-          <a:ext cx="7245000" cy="5956920"/>
+          <a:off x="77040" y="720"/>
+          <a:ext cx="7143120" cy="5956560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -417,11 +454,22 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0"/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1">
+            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
             <a:t>By default, imported accounts will inherit the default billing parameters set in Sonar. If you would like to override the default billing parameters with modified parameters, use this import.</a:t>
@@ -433,7 +481,12 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1">
+            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
             <a:t>Each column in the data tab has a note describing the format of the data.</a:t>
@@ -480,7 +533,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -499,24 +552,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.75510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.015306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.984693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.4285714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.8112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.1275510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.9744897959184"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -547,11 +601,17 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>